<commit_message>
Organizando dados na planilha
</commit_message>
<xml_diff>
--- a/ecommerce-meteora.xlsx
+++ b/ecommerce-meteora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gribeirodeal\cursos-alura\curso-excel-domine-editor-planilhas-alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4474B376-12DF-453E-838B-6384A74D2D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F33D9F-67B2-429A-86EF-B588C072BE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{6AB271C9-5D0E-4B15-8F38-762E3FE2F848}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6AB271C9-5D0E-4B15-8F38-762E3FE2F848}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Produtos</t>
   </si>
@@ -51,6 +51,27 @@
   </si>
   <si>
     <t>Óculos</t>
+  </si>
+  <si>
+    <t>Tamanho</t>
+  </si>
+  <si>
+    <t>Jaqueta</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Tênis</t>
+  </si>
+  <si>
+    <t>Bolsa</t>
+  </si>
+  <si>
+    <t>Boné</t>
+  </si>
+  <si>
+    <t>Cinto</t>
   </si>
 </sst>
 </file>
@@ -402,37 +423,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE12F67-A69D-4557-9949-60645819EA62}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>